<commit_message>
ultima versión de los gimnasios
</commit_message>
<xml_diff>
--- a/GYM_CUCUTA.xlsx
+++ b/GYM_CUCUTA.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\ANDROIDFIN\android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tini\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,21 +29,9 @@
     <t>GIMNASIOS DE CUCUTA</t>
   </si>
   <si>
-    <t>SUPER GIMNASIO LA 13</t>
-  </si>
-  <si>
-    <t>CALLE 13 2-61 CENTRO</t>
-  </si>
-  <si>
     <t xml:space="preserve">CACIQUE FITNNES </t>
   </si>
   <si>
-    <t>AV 2 16-01 LA PLAYA</t>
-  </si>
-  <si>
-    <t>7.884905, -72.498733</t>
-  </si>
-  <si>
     <t>7.881563, -72.499562</t>
   </si>
   <si>
@@ -101,9 +89,6 @@
     <t>#16- a, Cl. 10 #16-121 EL LLANO</t>
   </si>
   <si>
-    <t>Av. 1 Este #2022, Cúcuta, Norte de Santander</t>
-  </si>
-  <si>
     <t>7.877994, -72.496186</t>
   </si>
   <si>
@@ -134,9 +119,6 @@
     <t>Avenida 2E # 13- 21 LA LAGUNA</t>
   </si>
   <si>
-    <t>Av. 3 Este ## 14a, Cúcuta, Norte de Santander</t>
-  </si>
-  <si>
     <t>7.884312, -72.494593</t>
   </si>
   <si>
@@ -146,9 +128,6 @@
     <t>314 3207861</t>
   </si>
   <si>
-    <t>#8- a, Av. 10 #8125, Cúcuta, Norte de Santander</t>
-  </si>
-  <si>
     <t>7.887174, -72.509256</t>
   </si>
   <si>
@@ -189,13 +168,34 @@
   </si>
   <si>
     <t>CALLE 16N AV 0 EL BOSQUE</t>
+  </si>
+  <si>
+    <t>7.887723, -72.494997</t>
+  </si>
+  <si>
+    <t>BODY TECH</t>
+  </si>
+  <si>
+    <t>Cl. 11 #2E-10 caobos</t>
+  </si>
+  <si>
+    <t>AV 2 16-01 la playa</t>
+  </si>
+  <si>
+    <t>Av. 1 Este #2022 Barrio blanco</t>
+  </si>
+  <si>
+    <t>Av. 3 Este # 14a, Cúcuta, Norte de Santander</t>
+  </si>
+  <si>
+    <t>8- a, Av. 10 #8125, barrio llano</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +224,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -233,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -258,21 +264,6 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -433,48 +424,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,7 +745,7 @@
   <dimension ref="B1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,228 +760,228 @@
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E4" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="E5" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="E8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+      <c r="E10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="E11" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="E12" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="14" t="s">
+      <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="10"/>
       <c r="H14" s="4"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
-        <v>45</v>
+      <c r="B15" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="15"/>
+        <v>37</v>
+      </c>
+      <c r="E15" s="10"/>
       <c r="H15" s="3"/>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
-        <v>46</v>
+      <c r="B16" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
-        <v>53</v>
+      <c r="B17" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="15"/>
+        <v>45</v>
+      </c>
+      <c r="E17" s="10"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>